<commit_message>
Moved C59 and C60 to "C59-C72.R", worked on C59-72
</commit_message>
<xml_diff>
--- a/Doc/LCdatadictionary.xlsx
+++ b/Doc/LCdatadictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhnw365.sharepoint.com/teams/O365_G_DataScience_Admin/Freigegebene Dokumente/General/_2022/Slides/00-Group_Assignments/DATA/Part 1-Loans/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e87c79d324f92c85/Documents/R_Projects/FHNW_Data_Science/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="6" documentId="8_{56178724-7C99-4540-ADEA-7945BA418AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7249AF8-6F5D-854F-8C9D-E0CEAEB23116}"/>
   <bookViews>
-    <workbookView xWindow="-660" yWindow="-21140" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -1942,19 +1942,19 @@
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="196.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118.83203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="196.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118.85546875" style="6" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1980,7 +1980,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -2016,7 +2016,7 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -2034,7 +2034,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -2043,7 +2043,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
@@ -2052,7 +2052,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
@@ -2088,7 +2088,7 @@
       </c>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="4" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>32</v>
       </c>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>38</v>
       </c>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>40</v>
       </c>
@@ -2124,7 +2124,7 @@
       </c>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>42</v>
       </c>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>44</v>
       </c>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>46</v>
       </c>
@@ -2151,7 +2151,7 @@
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>48</v>
       </c>
@@ -2160,7 +2160,7 @@
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>50</v>
       </c>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>52</v>
       </c>
@@ -2178,7 +2178,7 @@
       </c>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:10" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>54</v>
       </c>
@@ -2187,7 +2187,7 @@
       </c>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>56</v>
       </c>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>58</v>
       </c>
@@ -2205,7 +2205,7 @@
       </c>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>60</v>
       </c>
@@ -2214,7 +2214,7 @@
       </c>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>62</v>
       </c>
@@ -2223,7 +2223,7 @@
       </c>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>64</v>
       </c>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>66</v>
       </c>
@@ -2243,7 +2243,7 @@
       <c r="I32" s="10"/>
       <c r="J32" s="11"/>
     </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>68</v>
       </c>
@@ -2252,7 +2252,7 @@
       </c>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>70</v>
       </c>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>72</v>
       </c>
@@ -2270,7 +2270,7 @@
       </c>
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>74</v>
       </c>
@@ -2279,7 +2279,7 @@
       </c>
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>76</v>
       </c>
@@ -2288,7 +2288,7 @@
       </c>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>78</v>
       </c>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>80</v>
       </c>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>82</v>
       </c>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>84</v>
       </c>
@@ -2327,7 +2327,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="11"/>
     </row>
-    <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>86</v>
       </c>
@@ -2339,7 +2339,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
     </row>
-    <row r="43" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>88</v>
       </c>
@@ -2351,7 +2351,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="11"/>
     </row>
-    <row r="44" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>90</v>
       </c>
@@ -2360,7 +2360,7 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>93</v>
       </c>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>95</v>
       </c>
@@ -2378,7 +2378,7 @@
       </c>
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>97</v>
       </c>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>99</v>
       </c>
@@ -2396,7 +2396,7 @@
       </c>
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>101</v>
       </c>
@@ -2405,7 +2405,7 @@
       </c>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>103</v>
       </c>
@@ -2414,7 +2414,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>105</v>
       </c>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>107</v>
       </c>
@@ -2432,7 +2432,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>109</v>
       </c>
@@ -2441,7 +2441,7 @@
       </c>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>111</v>
       </c>
@@ -2450,7 +2450,7 @@
       </c>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
         <v>113</v>
       </c>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>115</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>117</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>119</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>121</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>123</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>125</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>127</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>129</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>131</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>133</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>135</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>137</v>
       </c>
@@ -2557,7 +2557,7 @@
       <c r="C67"/>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>139</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>141</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>143</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>145</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>147</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>149</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B75" s="13" t="s">
         <v>151</v>
       </c>
@@ -2638,14 +2638,14 @@
       <selection pane="bottomLeft" activeCell="A87" sqref="A87:XFD87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="235.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="235.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="235.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="235.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>152</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>153</v>
       </c>
@@ -2664,7 +2664,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>155</v>
       </c>
@@ -2675,7 +2675,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>156</v>
       </c>
@@ -2686,7 +2686,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>158</v>
       </c>
@@ -2697,7 +2697,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>159</v>
       </c>
@@ -2715,7 +2715,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
@@ -2724,7 +2724,7 @@
       </c>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>160</v>
       </c>
@@ -2734,7 +2734,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>162</v>
       </c>
@@ -2745,7 +2745,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>164</v>
       </c>
@@ -2756,7 +2756,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>166</v>
       </c>
@@ -2766,7 +2766,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
@@ -2776,7 +2776,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>168</v>
       </c>
@@ -2787,7 +2787,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>170</v>
       </c>
@@ -2798,7 +2798,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>171</v>
       </c>
@@ -2809,7 +2809,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>16</v>
       </c>
@@ -2820,7 +2820,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
@@ -2831,7 +2831,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>20</v>
       </c>
@@ -2840,7 +2840,7 @@
       </c>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>173</v>
       </c>
@@ -2851,7 +2851,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>175</v>
       </c>
@@ -2861,7 +2861,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>26</v>
       </c>
@@ -2872,7 +2872,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>177</v>
       </c>
@@ -2883,7 +2883,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>179</v>
       </c>
@@ -2894,7 +2894,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>181</v>
       </c>
@@ -2905,7 +2905,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>183</v>
       </c>
@@ -2916,7 +2916,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>184</v>
       </c>
@@ -2927,7 +2927,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>185</v>
       </c>
@@ -2938,7 +2938,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>34</v>
       </c>
@@ -2949,7 +2949,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>186</v>
       </c>
@@ -2960,7 +2960,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>38</v>
       </c>
@@ -2971,7 +2971,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>187</v>
       </c>
@@ -2981,7 +2981,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>189</v>
       </c>
@@ -2991,7 +2991,7 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>190</v>
       </c>
@@ -3002,7 +3002,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -3013,7 +3013,7 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>191</v>
       </c>
@@ -3024,7 +3024,7 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>193</v>
       </c>
@@ -3035,7 +3035,7 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>194</v>
       </c>
@@ -3046,7 +3046,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>196</v>
       </c>
@@ -3057,7 +3057,7 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>197</v>
       </c>
@@ -3068,7 +3068,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>198</v>
       </c>
@@ -3078,7 +3078,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>200</v>
       </c>
@@ -3088,7 +3088,7 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>202</v>
       </c>
@@ -3098,7 +3098,7 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>204</v>
       </c>
@@ -3108,7 +3108,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>206</v>
       </c>
@@ -3118,7 +3118,7 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>66</v>
       </c>
@@ -3129,7 +3129,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>208</v>
       </c>
@@ -3139,7 +3139,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>210</v>
       </c>
@@ -3149,7 +3149,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>211</v>
       </c>
@@ -3159,7 +3159,7 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>212</v>
       </c>
@@ -3169,7 +3169,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>214</v>
       </c>
@@ -3179,7 +3179,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>216</v>
       </c>
@@ -3189,7 +3189,7 @@
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>218</v>
       </c>
@@ -3198,7 +3198,7 @@
       </c>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>220</v>
       </c>
@@ -3207,7 +3207,7 @@
       </c>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>222</v>
       </c>
@@ -3216,7 +3216,7 @@
       </c>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>224</v>
       </c>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>226</v>
       </c>
@@ -3234,7 +3234,7 @@
       </c>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>228</v>
       </c>
@@ -3243,7 +3243,7 @@
       </c>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>230</v>
       </c>
@@ -3252,7 +3252,7 @@
       </c>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>232</v>
       </c>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>234</v>
       </c>
@@ -3270,7 +3270,7 @@
       </c>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>236</v>
       </c>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>238</v>
       </c>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>240</v>
       </c>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>242</v>
       </c>
@@ -3306,7 +3306,7 @@
       </c>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>244</v>
       </c>
@@ -3315,7 +3315,7 @@
       </c>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>246</v>
       </c>
@@ -3324,7 +3324,7 @@
       </c>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>248</v>
       </c>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>249</v>
       </c>
@@ -3342,7 +3342,7 @@
       </c>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>251</v>
       </c>
@@ -3352,7 +3352,7 @@
       <c r="D70" s="6"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>253</v>
       </c>
@@ -3361,7 +3361,7 @@
       </c>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>255</v>
       </c>
@@ -3370,7 +3370,7 @@
       </c>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>82</v>
       </c>
@@ -3380,7 +3380,7 @@
       <c r="D73" s="6"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>256</v>
       </c>
@@ -3390,7 +3390,7 @@
       <c r="D74" s="6"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>258</v>
       </c>
@@ -3400,7 +3400,7 @@
       <c r="D75" s="6"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>260</v>
       </c>
@@ -3409,7 +3409,7 @@
       </c>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>261</v>
       </c>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>262</v>
       </c>
@@ -3428,7 +3428,7 @@
       <c r="D78" s="6"/>
       <c r="F78" s="6"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>264</v>
       </c>
@@ -3438,7 +3438,7 @@
       <c r="D79" s="6"/>
       <c r="F79" s="6"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>265</v>
       </c>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="F80" s="6"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>93</v>
       </c>
@@ -3457,7 +3457,7 @@
       <c r="D81" s="6"/>
       <c r="F81" s="6"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>95</v>
       </c>
@@ -3467,7 +3467,7 @@
       <c r="D82" s="6"/>
       <c r="F82" s="6"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>147</v>
       </c>
@@ -3476,7 +3476,7 @@
       </c>
       <c r="F83" s="6"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>149</v>
       </c>
@@ -3485,7 +3485,7 @@
       </c>
       <c r="F84" s="6"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>267</v>
       </c>
@@ -3494,7 +3494,7 @@
       </c>
       <c r="F85" s="6"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>269</v>
       </c>
@@ -3503,7 +3503,7 @@
       </c>
       <c r="F86" s="6"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>137</v>
       </c>
@@ -3512,7 +3512,7 @@
       </c>
       <c r="F87" s="6"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>271</v>
       </c>
@@ -3521,7 +3521,7 @@
       </c>
       <c r="F88" s="6"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>272</v>
       </c>
@@ -3530,7 +3530,7 @@
       </c>
       <c r="F89" s="6"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>274</v>
       </c>
@@ -3539,7 +3539,7 @@
       </c>
       <c r="F90" s="6"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>109</v>
       </c>
@@ -3549,7 +3549,7 @@
       <c r="D91" s="6"/>
       <c r="F91" s="6"/>
     </row>
-    <row r="92" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>111</v>
       </c>
@@ -3558,7 +3558,7 @@
       </c>
       <c r="D92"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="22" t="s">
         <v>113</v>
       </c>
@@ -3568,7 +3568,7 @@
       <c r="D93" s="6"/>
       <c r="F93" s="6"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>115</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>117</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>119</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>121</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>123</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>125</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>127</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>129</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>131</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>133</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>135</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>139</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>141</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>143</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B109" s="13" t="s">
         <v>151</v>
       </c>
@@ -3712,13 +3712,13 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="225.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="225.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>276</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>277</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>279</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>281</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>282</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>284</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>285</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>286</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>287</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>288</v>
       </c>
@@ -3798,11 +3798,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
     </row>
@@ -3819,6 +3819,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b4a7e659-09bd-4686-945b-72100c560ea7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1f70f612-e078-4a38-9ca6-da83905434d6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004C68B603FDEE62438157E9DC6731ACFB" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="90e67d3b1e083a7c68dd0f6a2dbfa958">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1f70f612-e078-4a38-9ca6-da83905434d6" xmlns:ns3="b4a7e659-09bd-4686-945b-72100c560ea7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="053fbf71ecc4d66dde3b044e8477e22d" ns2:_="" ns3:_="">
     <xsd:import namespace="1f70f612-e078-4a38-9ca6-da83905434d6"/>
@@ -4061,28 +4081,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b4a7e659-09bd-4686-945b-72100c560ea7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1f70f612-e078-4a38-9ca6-da83905434d6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB070A2D-5B3A-40DE-B49C-F3CC431F704D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E045B5B-9298-4CA2-B8A8-8516AD835D96}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1f70f612-e078-4a38-9ca6-da83905434d6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="b4a7e659-09bd-4686-945b-72100c560ea7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4094,17 +4107,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E045B5B-9298-4CA2-B8A8-8516AD835D96}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB070A2D-5B3A-40DE-B49C-F3CC431F704D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1f70f612-e078-4a38-9ca6-da83905434d6"/>
+    <ds:schemaRef ds:uri="b4a7e659-09bd-4686-945b-72100c560ea7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1f70f612-e078-4a38-9ca6-da83905434d6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Moved C59 and C60 to "C59-C72.R", added Data Cleanup
</commit_message>
<xml_diff>
--- a/Doc/LCdatadictionary.xlsx
+++ b/Doc/LCdatadictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhnw365.sharepoint.com/teams/O365_G_DataScience_Admin/Freigegebene Dokumente/General/_2022/Slides/00-Group_Assignments/DATA/Part 1-Loans/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e87c79d324f92c85/Documents/R_Projects/FHNW_Data_Science/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="6" documentId="8_{56178724-7C99-4540-ADEA-7945BA418AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7249AF8-6F5D-854F-8C9D-E0CEAEB23116}"/>
   <bookViews>
-    <workbookView xWindow="-660" yWindow="-21140" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -1942,19 +1942,19 @@
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="196.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118.83203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="196.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118.85546875" style="6" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1980,7 +1980,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -2016,7 +2016,7 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -2034,7 +2034,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -2043,7 +2043,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
@@ -2052,7 +2052,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
@@ -2088,7 +2088,7 @@
       </c>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="4" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>32</v>
       </c>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>38</v>
       </c>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>40</v>
       </c>
@@ -2124,7 +2124,7 @@
       </c>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>42</v>
       </c>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>44</v>
       </c>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>46</v>
       </c>
@@ -2151,7 +2151,7 @@
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>48</v>
       </c>
@@ -2160,7 +2160,7 @@
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>50</v>
       </c>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>52</v>
       </c>
@@ -2178,7 +2178,7 @@
       </c>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:10" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>54</v>
       </c>
@@ -2187,7 +2187,7 @@
       </c>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>56</v>
       </c>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>58</v>
       </c>
@@ -2205,7 +2205,7 @@
       </c>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>60</v>
       </c>
@@ -2214,7 +2214,7 @@
       </c>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>62</v>
       </c>
@@ -2223,7 +2223,7 @@
       </c>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>64</v>
       </c>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>66</v>
       </c>
@@ -2243,7 +2243,7 @@
       <c r="I32" s="10"/>
       <c r="J32" s="11"/>
     </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>68</v>
       </c>
@@ -2252,7 +2252,7 @@
       </c>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>70</v>
       </c>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>72</v>
       </c>
@@ -2270,7 +2270,7 @@
       </c>
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>74</v>
       </c>
@@ -2279,7 +2279,7 @@
       </c>
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>76</v>
       </c>
@@ -2288,7 +2288,7 @@
       </c>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>78</v>
       </c>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>80</v>
       </c>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>82</v>
       </c>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>84</v>
       </c>
@@ -2327,7 +2327,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="11"/>
     </row>
-    <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>86</v>
       </c>
@@ -2339,7 +2339,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
     </row>
-    <row r="43" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>88</v>
       </c>
@@ -2351,7 +2351,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="11"/>
     </row>
-    <row r="44" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>90</v>
       </c>
@@ -2360,7 +2360,7 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>93</v>
       </c>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>95</v>
       </c>
@@ -2378,7 +2378,7 @@
       </c>
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>97</v>
       </c>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>99</v>
       </c>
@@ -2396,7 +2396,7 @@
       </c>
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>101</v>
       </c>
@@ -2405,7 +2405,7 @@
       </c>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>103</v>
       </c>
@@ -2414,7 +2414,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>105</v>
       </c>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>107</v>
       </c>
@@ -2432,7 +2432,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>109</v>
       </c>
@@ -2441,7 +2441,7 @@
       </c>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>111</v>
       </c>
@@ -2450,7 +2450,7 @@
       </c>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
         <v>113</v>
       </c>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>115</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>117</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>119</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>121</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>123</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>125</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>127</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>129</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>131</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>133</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>135</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>137</v>
       </c>
@@ -2557,7 +2557,7 @@
       <c r="C67"/>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>139</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>141</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>143</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>145</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>147</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>149</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B75" s="13" t="s">
         <v>151</v>
       </c>
@@ -2638,14 +2638,14 @@
       <selection pane="bottomLeft" activeCell="A87" sqref="A87:XFD87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="235.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="235.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="235.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="235.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>152</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>153</v>
       </c>
@@ -2664,7 +2664,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>155</v>
       </c>
@@ -2675,7 +2675,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>156</v>
       </c>
@@ -2686,7 +2686,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>158</v>
       </c>
@@ -2697,7 +2697,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>159</v>
       </c>
@@ -2715,7 +2715,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
@@ -2724,7 +2724,7 @@
       </c>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>160</v>
       </c>
@@ -2734,7 +2734,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>162</v>
       </c>
@@ -2745,7 +2745,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>164</v>
       </c>
@@ -2756,7 +2756,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>166</v>
       </c>
@@ -2766,7 +2766,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
@@ -2776,7 +2776,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>168</v>
       </c>
@@ -2787,7 +2787,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>170</v>
       </c>
@@ -2798,7 +2798,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>171</v>
       </c>
@@ -2809,7 +2809,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>16</v>
       </c>
@@ -2820,7 +2820,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
@@ -2831,7 +2831,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>20</v>
       </c>
@@ -2840,7 +2840,7 @@
       </c>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>173</v>
       </c>
@@ -2851,7 +2851,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>175</v>
       </c>
@@ -2861,7 +2861,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>26</v>
       </c>
@@ -2872,7 +2872,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>177</v>
       </c>
@@ -2883,7 +2883,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>179</v>
       </c>
@@ -2894,7 +2894,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>181</v>
       </c>
@@ -2905,7 +2905,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>183</v>
       </c>
@@ -2916,7 +2916,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>184</v>
       </c>
@@ -2927,7 +2927,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>185</v>
       </c>
@@ -2938,7 +2938,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>34</v>
       </c>
@@ -2949,7 +2949,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>186</v>
       </c>
@@ -2960,7 +2960,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>38</v>
       </c>
@@ -2971,7 +2971,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>187</v>
       </c>
@@ -2981,7 +2981,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>189</v>
       </c>
@@ -2991,7 +2991,7 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>190</v>
       </c>
@@ -3002,7 +3002,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -3013,7 +3013,7 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>191</v>
       </c>
@@ -3024,7 +3024,7 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>193</v>
       </c>
@@ -3035,7 +3035,7 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>194</v>
       </c>
@@ -3046,7 +3046,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>196</v>
       </c>
@@ -3057,7 +3057,7 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>197</v>
       </c>
@@ -3068,7 +3068,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>198</v>
       </c>
@@ -3078,7 +3078,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>200</v>
       </c>
@@ -3088,7 +3088,7 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>202</v>
       </c>
@@ -3098,7 +3098,7 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>204</v>
       </c>
@@ -3108,7 +3108,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>206</v>
       </c>
@@ -3118,7 +3118,7 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>66</v>
       </c>
@@ -3129,7 +3129,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>208</v>
       </c>
@@ -3139,7 +3139,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>210</v>
       </c>
@@ -3149,7 +3149,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>211</v>
       </c>
@@ -3159,7 +3159,7 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>212</v>
       </c>
@@ -3169,7 +3169,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>214</v>
       </c>
@@ -3179,7 +3179,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>216</v>
       </c>
@@ -3189,7 +3189,7 @@
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>218</v>
       </c>
@@ -3198,7 +3198,7 @@
       </c>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>220</v>
       </c>
@@ -3207,7 +3207,7 @@
       </c>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>222</v>
       </c>
@@ -3216,7 +3216,7 @@
       </c>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>224</v>
       </c>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>226</v>
       </c>
@@ -3234,7 +3234,7 @@
       </c>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>228</v>
       </c>
@@ -3243,7 +3243,7 @@
       </c>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>230</v>
       </c>
@@ -3252,7 +3252,7 @@
       </c>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>232</v>
       </c>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>234</v>
       </c>
@@ -3270,7 +3270,7 @@
       </c>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>236</v>
       </c>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>238</v>
       </c>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>240</v>
       </c>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>242</v>
       </c>
@@ -3306,7 +3306,7 @@
       </c>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>244</v>
       </c>
@@ -3315,7 +3315,7 @@
       </c>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>246</v>
       </c>
@@ -3324,7 +3324,7 @@
       </c>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>248</v>
       </c>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>249</v>
       </c>
@@ -3342,7 +3342,7 @@
       </c>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>251</v>
       </c>
@@ -3352,7 +3352,7 @@
       <c r="D70" s="6"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>253</v>
       </c>
@@ -3361,7 +3361,7 @@
       </c>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>255</v>
       </c>
@@ -3370,7 +3370,7 @@
       </c>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>82</v>
       </c>
@@ -3380,7 +3380,7 @@
       <c r="D73" s="6"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>256</v>
       </c>
@@ -3390,7 +3390,7 @@
       <c r="D74" s="6"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>258</v>
       </c>
@@ -3400,7 +3400,7 @@
       <c r="D75" s="6"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>260</v>
       </c>
@@ -3409,7 +3409,7 @@
       </c>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>261</v>
       </c>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>262</v>
       </c>
@@ -3428,7 +3428,7 @@
       <c r="D78" s="6"/>
       <c r="F78" s="6"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>264</v>
       </c>
@@ -3438,7 +3438,7 @@
       <c r="D79" s="6"/>
       <c r="F79" s="6"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>265</v>
       </c>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="F80" s="6"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>93</v>
       </c>
@@ -3457,7 +3457,7 @@
       <c r="D81" s="6"/>
       <c r="F81" s="6"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>95</v>
       </c>
@@ -3467,7 +3467,7 @@
       <c r="D82" s="6"/>
       <c r="F82" s="6"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>147</v>
       </c>
@@ -3476,7 +3476,7 @@
       </c>
       <c r="F83" s="6"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>149</v>
       </c>
@@ -3485,7 +3485,7 @@
       </c>
       <c r="F84" s="6"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>267</v>
       </c>
@@ -3494,7 +3494,7 @@
       </c>
       <c r="F85" s="6"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>269</v>
       </c>
@@ -3503,7 +3503,7 @@
       </c>
       <c r="F86" s="6"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>137</v>
       </c>
@@ -3512,7 +3512,7 @@
       </c>
       <c r="F87" s="6"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>271</v>
       </c>
@@ -3521,7 +3521,7 @@
       </c>
       <c r="F88" s="6"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>272</v>
       </c>
@@ -3530,7 +3530,7 @@
       </c>
       <c r="F89" s="6"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>274</v>
       </c>
@@ -3539,7 +3539,7 @@
       </c>
       <c r="F90" s="6"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>109</v>
       </c>
@@ -3549,7 +3549,7 @@
       <c r="D91" s="6"/>
       <c r="F91" s="6"/>
     </row>
-    <row r="92" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>111</v>
       </c>
@@ -3558,7 +3558,7 @@
       </c>
       <c r="D92"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="22" t="s">
         <v>113</v>
       </c>
@@ -3568,7 +3568,7 @@
       <c r="D93" s="6"/>
       <c r="F93" s="6"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>115</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>117</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>119</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>121</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>123</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>125</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>127</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>129</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>131</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>133</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>135</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>139</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>141</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>143</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B109" s="13" t="s">
         <v>151</v>
       </c>
@@ -3712,13 +3712,13 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="225.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="225.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>276</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>277</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>279</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>281</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>282</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>284</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>285</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>286</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>287</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>288</v>
       </c>
@@ -3798,11 +3798,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
     </row>
@@ -3819,6 +3819,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b4a7e659-09bd-4686-945b-72100c560ea7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1f70f612-e078-4a38-9ca6-da83905434d6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004C68B603FDEE62438157E9DC6731ACFB" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="90e67d3b1e083a7c68dd0f6a2dbfa958">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1f70f612-e078-4a38-9ca6-da83905434d6" xmlns:ns3="b4a7e659-09bd-4686-945b-72100c560ea7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="053fbf71ecc4d66dde3b044e8477e22d" ns2:_="" ns3:_="">
     <xsd:import namespace="1f70f612-e078-4a38-9ca6-da83905434d6"/>
@@ -4061,28 +4081,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b4a7e659-09bd-4686-945b-72100c560ea7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1f70f612-e078-4a38-9ca6-da83905434d6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB070A2D-5B3A-40DE-B49C-F3CC431F704D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E045B5B-9298-4CA2-B8A8-8516AD835D96}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1f70f612-e078-4a38-9ca6-da83905434d6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="b4a7e659-09bd-4686-945b-72100c560ea7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4094,17 +4107,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E045B5B-9298-4CA2-B8A8-8516AD835D96}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB070A2D-5B3A-40DE-B49C-F3CC431F704D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1f70f612-e078-4a38-9ca6-da83905434d6"/>
+    <ds:schemaRef ds:uri="b4a7e659-09bd-4686-945b-72100c560ea7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1f70f612-e078-4a38-9ca6-da83905434d6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>